<commit_message>
AT: script changes to omit "Other" land from statistics
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
@@ -10,6 +10,74 @@
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>CRPland_acresk</t>
+  </si>
+  <si>
+    <t>Cropland_acresk</t>
+  </si>
+  <si>
+    <t>Forestland_acresk</t>
+  </si>
+  <si>
+    <t>NA_acresk</t>
+  </si>
+  <si>
+    <t>Otherland_acresk</t>
+  </si>
+  <si>
+    <t>Pastureland_acresk</t>
+  </si>
+  <si>
+    <t>Rangeland_acresk</t>
+  </si>
+  <si>
+    <t>Urbanland_acresk</t>
+  </si>
+  <si>
+    <t>lccL1_acresk</t>
+  </si>
+  <si>
+    <t>lccL2_acresk</t>
+  </si>
+  <si>
+    <t>lccL3_acresk</t>
+  </si>
+  <si>
+    <t>lccL4_acresk</t>
+  </si>
+  <si>
+    <t>lccL5_acresk</t>
+  </si>
+  <si>
+    <t>lccL6_acresk</t>
+  </si>
+  <si>
+    <t>lccL7_acresk</t>
+  </si>
+  <si>
+    <t>lccL8_acresk</t>
+  </si>
+  <si>
+    <t>lccL12_acresk</t>
+  </si>
+  <si>
+    <t>lccL34_acresk</t>
+  </si>
+  <si>
+    <t>lccL56_acresk</t>
+  </si>
+  <si>
+    <t>lccL78_acresk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53,461 +121,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
-        <v>1982</v>
-      </c>
-      <c r="B1" s="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>366293.80031781644</v>
-      </c>
-      <c r="D1" s="1">
-        <v>408769.80038847774</v>
-      </c>
-      <c r="E1" s="1">
-        <v>397162.80126878619</v>
-      </c>
-      <c r="F1" s="1">
-        <v>112054.60072848201</v>
-      </c>
-      <c r="G1" s="1">
-        <v>183682.79997011274</v>
-      </c>
-      <c r="H1" s="1">
-        <v>417288.4997985065</v>
-      </c>
-      <c r="I1" s="1">
-        <v>50395.500189445913</v>
-      </c>
-      <c r="J1" s="1">
-        <v>29415.900061555207</v>
-      </c>
-      <c r="K1" s="1">
-        <v>285804.70041872561</v>
-      </c>
-      <c r="L1" s="1">
-        <v>287258.20014818013</v>
-      </c>
-      <c r="M1" s="1">
-        <v>201368.19981963933</v>
-      </c>
-      <c r="N1" s="1">
-        <v>34436.700032874942</v>
-      </c>
-      <c r="O1" s="1">
-        <v>280848.29983764142</v>
-      </c>
-      <c r="P1" s="1">
-        <v>274476.90060616285</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>23673.200044490397</v>
-      </c>
-      <c r="R1" s="1">
-        <v>315220.60089789331</v>
-      </c>
-      <c r="S1" s="1">
-        <v>488626.39942798018</v>
-      </c>
-      <c r="T1" s="1">
-        <v>315284.99992906302</v>
-      </c>
-      <c r="U1" s="1">
-        <v>298150.10048868507</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1987</v>
+        <v>1982</v>
       </c>
       <c r="B2" s="1">
-        <v>13776.799965359271</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>347130.90032412857</v>
+        <v>366293.80031781644</v>
       </c>
       <c r="D2" s="1">
-        <v>410698.30034087598</v>
+        <v>408769.80038847774</v>
       </c>
       <c r="E2" s="1">
-        <v>397583.60126296431</v>
+        <v>397162.80126878619</v>
       </c>
       <c r="F2" s="1">
-        <v>113429.90074026585</v>
+        <v>112054.60072848201</v>
       </c>
       <c r="G2" s="1">
-        <v>184756.0999750942</v>
+        <v>183682.79997011274</v>
       </c>
       <c r="H2" s="1">
-        <v>411972.79980929196</v>
+        <v>417288.4997985065</v>
       </c>
       <c r="I2" s="1">
-        <v>56299.400243647397</v>
+        <v>50395.500189445913</v>
       </c>
       <c r="J2" s="1">
-        <v>29203.800061307847</v>
+        <v>29415.900061555207</v>
       </c>
       <c r="K2" s="1">
-        <v>283727.80040160567</v>
+        <v>285804.70041872561</v>
       </c>
       <c r="L2" s="1">
-        <v>285858.70012959838</v>
+        <v>287258.20014818013</v>
       </c>
       <c r="M2" s="1">
-        <v>200138.29981394112</v>
+        <v>201368.19981963933</v>
       </c>
       <c r="N2" s="1">
-        <v>34214.70003335923</v>
+        <v>34436.700032874942</v>
       </c>
       <c r="O2" s="1">
-        <v>279713.99981605262</v>
+        <v>280848.29983764142</v>
       </c>
       <c r="P2" s="1">
-        <v>273535.60060277581</v>
+        <v>274476.90060616285</v>
       </c>
       <c r="Q2" s="1">
-        <v>23499.100045084953</v>
+        <v>23673.200044490397</v>
       </c>
       <c r="R2" s="1">
-        <v>312931.60042268783</v>
+        <v>315220.60089789331</v>
       </c>
       <c r="S2" s="1">
-        <v>485996.99948277324</v>
+        <v>488626.39942798018</v>
       </c>
       <c r="T2" s="1">
-        <v>313928.69983317703</v>
+        <v>315284.99992906302</v>
       </c>
       <c r="U2" s="1">
-        <v>297034.70043640584</v>
+        <v>298150.10048868507</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B3" s="1">
-        <v>34028.89997445792</v>
+        <v>13776.799965359271</v>
       </c>
       <c r="C3" s="1">
-        <v>326180.80028748512</v>
+        <v>347130.90032412857</v>
       </c>
       <c r="D3" s="1">
-        <v>410724.00032814592</v>
+        <v>410698.30034087598</v>
       </c>
       <c r="E3" s="1">
-        <v>399704.90127181262</v>
+        <v>397583.60126296431</v>
       </c>
       <c r="F3" s="1">
-        <v>113724.40074580908</v>
+        <v>113429.90074026585</v>
       </c>
       <c r="G3" s="1">
-        <v>179640.79995769262</v>
+        <v>184756.0999750942</v>
       </c>
       <c r="H3" s="1">
-        <v>408321.59979435056</v>
+        <v>411972.79980929196</v>
       </c>
       <c r="I3" s="1">
-        <v>63322.400301873684</v>
+        <v>56299.400243647397</v>
       </c>
       <c r="J3" s="1">
-        <v>28958.700062960386</v>
+        <v>29203.800061307847</v>
       </c>
       <c r="K3" s="1">
-        <v>281252.10037818551</v>
+        <v>283727.80040160567</v>
       </c>
       <c r="L3" s="1">
-        <v>283776.60011488944</v>
+        <v>285858.70012959838</v>
       </c>
       <c r="M3" s="1">
-        <v>198597.5997979939</v>
+        <v>200138.29981394112</v>
       </c>
       <c r="N3" s="1">
-        <v>33955.300028540194</v>
+        <v>34214.70003335923</v>
       </c>
       <c r="O3" s="1">
-        <v>278276.49980251491</v>
+        <v>279713.99981605262</v>
       </c>
       <c r="P3" s="1">
-        <v>272506.50057555735</v>
+        <v>273535.60060277581</v>
       </c>
       <c r="Q3" s="1">
-        <v>23368.700041651726</v>
+        <v>23499.100045084953</v>
       </c>
       <c r="R3" s="1">
-        <v>310210.80069301277</v>
+        <v>312931.60042268783</v>
       </c>
       <c r="S3" s="1">
-        <v>482374.19978109002</v>
+        <v>485996.99948277324</v>
       </c>
       <c r="T3" s="1">
-        <v>312231.80042778701</v>
+        <v>313928.69983317703</v>
       </c>
       <c r="U3" s="1">
-        <v>295875.20085892081</v>
+        <v>297034.70043640584</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>1997</v>
+        <v>1992</v>
       </c>
       <c r="B4" s="1">
-        <v>32694.799968130887</v>
+        <v>34028.89997445792</v>
       </c>
       <c r="C4" s="1">
-        <v>318596.90027798712</v>
+        <v>326180.80028748512</v>
       </c>
       <c r="D4" s="1">
-        <v>411963.70026227832</v>
+        <v>410724.00032814592</v>
       </c>
       <c r="E4" s="1">
-        <v>400059.90127716959</v>
+        <v>399704.90127181262</v>
       </c>
       <c r="F4" s="1">
-        <v>114703.30075372756</v>
+        <v>113724.40074580908</v>
       </c>
       <c r="G4" s="1">
-        <v>176979.79991899431</v>
+        <v>179640.79995769262</v>
       </c>
       <c r="H4" s="1">
-        <v>406921.39978945255</v>
+        <v>408321.59979435056</v>
       </c>
       <c r="I4" s="1">
-        <v>73728.000413887203</v>
+        <v>63322.400301873684</v>
       </c>
       <c r="J4" s="1">
-        <v>28614.100060492754</v>
+        <v>28958.700062960386</v>
       </c>
       <c r="K4" s="1">
-        <v>278231.90034101903</v>
+        <v>281252.10037818551</v>
       </c>
       <c r="L4" s="1">
-        <v>281246.70008831471</v>
+        <v>283776.60011488944</v>
       </c>
       <c r="M4" s="1">
-        <v>196635.19977666438</v>
+        <v>198597.5997979939</v>
       </c>
       <c r="N4" s="1">
-        <v>33697.600026026368</v>
+        <v>33955.300028540194</v>
       </c>
       <c r="O4" s="1">
-        <v>276691.09979146719</v>
+        <v>278276.49980251491</v>
       </c>
       <c r="P4" s="1">
-        <v>271132.90056282282</v>
+        <v>272506.50057555735</v>
       </c>
       <c r="Q4" s="1">
-        <v>23137.500039316714</v>
+        <v>23368.700041651726</v>
       </c>
       <c r="R4" s="1">
-        <v>306846.00032241642</v>
+        <v>310210.80069301277</v>
       </c>
       <c r="S4" s="1">
-        <v>477881.89992043376</v>
+        <v>482374.19978109002</v>
       </c>
       <c r="T4" s="1">
-        <v>310388.7001921609</v>
+        <v>312231.80042778701</v>
       </c>
       <c r="U4" s="1">
-        <v>294270.40080493689</v>
+        <v>295875.20085892081</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="B5" s="1">
-        <v>31479.299961820245</v>
+        <v>32694.799968130887</v>
       </c>
       <c r="C5" s="1">
-        <v>303946.70026582479</v>
+        <v>318596.90027798712</v>
       </c>
       <c r="D5" s="1">
-        <v>412413.70020762086</v>
+        <v>411963.70026227832</v>
       </c>
       <c r="E5" s="1">
-        <v>401609.20130158961</v>
+        <v>400059.90127716959</v>
       </c>
       <c r="F5" s="1">
-        <v>115343.10075476021</v>
+        <v>114703.30075372756</v>
       </c>
       <c r="G5" s="1">
-        <v>182246.49990992248</v>
+        <v>176979.79991899431</v>
       </c>
       <c r="H5" s="1">
-        <v>406378.49974918365</v>
+        <v>406921.39978945255</v>
       </c>
       <c r="I5" s="1">
-        <v>82230.800510905683</v>
+        <v>73728.000413887203</v>
       </c>
       <c r="J5" s="1">
-        <v>28167.500054322183</v>
+        <v>28614.100060492754</v>
       </c>
       <c r="K5" s="1">
-        <v>275477.20031578839</v>
+        <v>278231.90034101903</v>
       </c>
       <c r="L5" s="1">
-        <v>278901.50006436557</v>
+        <v>281246.70008831471</v>
       </c>
       <c r="M5" s="1">
-        <v>195199.49975059181</v>
+        <v>196635.19977666438</v>
       </c>
       <c r="N5" s="1">
-        <v>33458.700022481382</v>
+        <v>33697.600026026368</v>
       </c>
       <c r="O5" s="1">
-        <v>275395.89978072792</v>
+        <v>276691.09979146719</v>
       </c>
       <c r="P5" s="1">
-        <v>268967.10051334649</v>
+        <v>271132.90056282282</v>
       </c>
       <c r="Q5" s="1">
-        <v>23043.400038696826</v>
+        <v>23137.500039316714</v>
       </c>
       <c r="R5" s="1">
-        <v>303644.70055441558</v>
+        <v>306846.00032241642</v>
       </c>
       <c r="S5" s="1">
-        <v>474101.00040176511</v>
+        <v>477881.89992043376</v>
       </c>
       <c r="T5" s="1">
-        <v>308854.59972546995</v>
+        <v>310388.7001921609</v>
       </c>
       <c r="U5" s="1">
-        <v>292010.50020884722</v>
+        <v>294270.40080493689</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="B6" s="1">
-        <v>32578.7999650985</v>
+        <v>31479.299961820245</v>
       </c>
       <c r="C6" s="1">
-        <v>298823.5002399534</v>
+        <v>303946.70026582479</v>
       </c>
       <c r="D6" s="1">
-        <v>412162.40016037226</v>
+        <v>412413.70020762086</v>
       </c>
       <c r="E6" s="1">
-        <v>402130.50130251795</v>
+        <v>401609.20130158961</v>
       </c>
       <c r="F6" s="1">
-        <v>117217.00075599551</v>
+        <v>115343.10075476021</v>
       </c>
       <c r="G6" s="1">
-        <v>179396.29990192503</v>
+        <v>182246.49990992248</v>
       </c>
       <c r="H6" s="1">
-        <v>405568.39974284917</v>
+        <v>406378.49974918365</v>
       </c>
       <c r="I6" s="1">
-        <v>87770.900592915714</v>
+        <v>82230.800510905683</v>
       </c>
       <c r="J6" s="1">
-        <v>27857.100053675473</v>
+        <v>28167.500054322183</v>
       </c>
       <c r="K6" s="1">
-        <v>273569.40028021485</v>
+        <v>275477.20031578839</v>
       </c>
       <c r="L6" s="1">
-        <v>277538.100043796</v>
+        <v>278901.50006436557</v>
       </c>
       <c r="M6" s="1">
-        <v>194130.29973341525</v>
+        <v>195199.49975059181</v>
       </c>
       <c r="N6" s="1">
-        <v>33300.300020866096</v>
+        <v>33458.700022481382</v>
       </c>
       <c r="O6" s="1">
-        <v>274717.89976213127</v>
+        <v>275395.89978072792</v>
       </c>
       <c r="P6" s="1">
-        <v>267977.70051269233</v>
+        <v>268967.10051334649</v>
       </c>
       <c r="Q6" s="1">
-        <v>22968.100036777556</v>
+        <v>23043.400038696826</v>
       </c>
       <c r="R6" s="1">
-        <v>301426.50051239133</v>
+        <v>303644.70055441558</v>
       </c>
       <c r="S6" s="1">
-        <v>471668.39942433685</v>
+        <v>474101.00040176511</v>
       </c>
       <c r="T6" s="1">
-        <v>308018.19972027093</v>
+        <v>308854.59972546995</v>
       </c>
       <c r="U6" s="1">
-        <v>290945.80068060756</v>
+        <v>292010.50020884722</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32578.7999650985</v>
+      </c>
+      <c r="C7" s="1">
+        <v>298823.5002399534</v>
+      </c>
+      <c r="D7" s="1">
+        <v>412162.40016037226</v>
+      </c>
+      <c r="E7" s="1">
+        <v>402130.50130251795</v>
+      </c>
+      <c r="F7" s="1">
+        <v>117217.00075599551</v>
+      </c>
+      <c r="G7" s="1">
+        <v>179396.29990192503</v>
+      </c>
+      <c r="H7" s="1">
+        <v>405568.39974284917</v>
+      </c>
+      <c r="I7" s="1">
+        <v>87770.900592915714</v>
+      </c>
+      <c r="J7" s="1">
+        <v>27857.100053675473</v>
+      </c>
+      <c r="K7" s="1">
+        <v>273569.40028021485</v>
+      </c>
+      <c r="L7" s="1">
+        <v>277538.100043796</v>
+      </c>
+      <c r="M7" s="1">
+        <v>194130.29973341525</v>
+      </c>
+      <c r="N7" s="1">
+        <v>33300.300020866096</v>
+      </c>
+      <c r="O7" s="1">
+        <v>274717.89976213127</v>
+      </c>
+      <c r="P7" s="1">
+        <v>267977.70051269233</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>22968.100036777556</v>
+      </c>
+      <c r="R7" s="1">
+        <v>301426.50051239133</v>
+      </c>
+      <c r="S7" s="1">
+        <v>471668.39942433685</v>
+      </c>
+      <c r="T7" s="1">
+        <v>308018.19972027093</v>
+      </c>
+      <c r="U7" s="1">
+        <v>290945.80068060756</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
         <v>2012</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>23949.599969789386</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>307765.8002416268</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>412705.60012216866</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>402616.90131063014</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>118212.60076145828</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>175692.29988637567</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H8" s="1">
         <v>404044.5997281298</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I8" s="1">
         <v>90660.400641448796</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J8" s="1">
         <v>27692.400049224496</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K8" s="1">
         <v>272671.80026450753</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L8" s="1">
         <v>276709.90002723038</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M8" s="1">
         <v>193570.89972167462</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N8" s="1">
         <v>33232.800019867718</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O8" s="1">
         <v>274218.79975289851</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P8" s="1">
         <v>267305.10050263256</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q8" s="1">
         <v>22970.000036463141</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R8" s="1">
         <v>300364.2005763948</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S8" s="1">
         <v>470280.80000023544</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T8" s="1">
         <v>307451.59990778565</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U8" s="1">
         <v>290275.10016013682</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AT: additional panel/sum statistics revisions, specifically excluding other and N/A from percentage calculations for both landu and LCC
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>year</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Forestland_acresk</t>
   </si>
   <si>
-    <t>NA_acresk</t>
+    <t>NAland_acresk</t>
   </si>
   <si>
     <t>Otherland_acresk</t>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Urbanland_acresk</t>
+  </si>
+  <si>
+    <t>lccNA_acresk</t>
   </si>
   <si>
     <t>lccL1_acresk</t>
@@ -121,7 +124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -188,6 +191,9 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -197,61 +203,64 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>366293.80031781644</v>
+        <v>366293.8001255244</v>
       </c>
       <c r="D2" s="1">
-        <v>408769.80038847774</v>
+        <v>408769.80048586428</v>
       </c>
       <c r="E2" s="1">
-        <v>397162.80126878619</v>
+        <v>397162.801202178</v>
       </c>
       <c r="F2" s="1">
-        <v>112054.60072848201</v>
+        <v>112054.60071638972</v>
       </c>
       <c r="G2" s="1">
-        <v>183682.79997011274</v>
+        <v>183682.80005792528</v>
       </c>
       <c r="H2" s="1">
-        <v>417288.4997985065</v>
+        <v>417288.50006688386</v>
       </c>
       <c r="I2" s="1">
-        <v>50395.500189445913</v>
+        <v>50395.500235527754</v>
       </c>
       <c r="J2" s="1">
-        <v>29415.900061555207</v>
+        <v>518365.7019867152</v>
       </c>
       <c r="K2" s="1">
-        <v>285804.70041872561</v>
+        <v>29415.90003991127</v>
       </c>
       <c r="L2" s="1">
-        <v>287258.20014818013</v>
+        <v>285804.70027589798</v>
       </c>
       <c r="M2" s="1">
-        <v>201368.19981963933</v>
+        <v>287258.20012904704</v>
       </c>
       <c r="N2" s="1">
-        <v>34436.700032874942</v>
+        <v>201368.20010298491</v>
       </c>
       <c r="O2" s="1">
-        <v>280848.29983764142</v>
+        <v>34436.700000435114</v>
       </c>
       <c r="P2" s="1">
-        <v>274476.90060616285</v>
+        <v>280848.30010822415</v>
       </c>
       <c r="Q2" s="1">
-        <v>23673.200044490397</v>
+        <v>274476.90023375303</v>
       </c>
       <c r="R2" s="1">
-        <v>315220.60089789331</v>
+        <v>23673.200013324618</v>
       </c>
       <c r="S2" s="1">
-        <v>488626.39942798018</v>
+        <v>315220.60031580925</v>
       </c>
       <c r="T2" s="1">
-        <v>315284.99992906302</v>
+        <v>488626.40023203194</v>
       </c>
       <c r="U2" s="1">
-        <v>298150.10048868507</v>
+        <v>315285.00010865927</v>
+      </c>
+      <c r="V2" s="1">
+        <v>298150.10024707764</v>
       </c>
     </row>
     <row r="3">
@@ -259,64 +268,67 @@
         <v>1987</v>
       </c>
       <c r="B3" s="1">
-        <v>13776.799965359271</v>
+        <v>13776.79998434335</v>
       </c>
       <c r="C3" s="1">
-        <v>347130.90032412857</v>
+        <v>347130.90011132509</v>
       </c>
       <c r="D3" s="1">
-        <v>410698.30034087598</v>
+        <v>410698.3004591614</v>
       </c>
       <c r="E3" s="1">
-        <v>397583.60126296431</v>
+        <v>397583.60121012479</v>
       </c>
       <c r="F3" s="1">
-        <v>113429.90074026585</v>
+        <v>113429.90072029084</v>
       </c>
       <c r="G3" s="1">
-        <v>184756.0999750942</v>
+        <v>184756.10005189478</v>
       </c>
       <c r="H3" s="1">
-        <v>411972.79980929196</v>
+        <v>411972.80007003248</v>
       </c>
       <c r="I3" s="1">
-        <v>56299.400243647397</v>
+        <v>56299.400283120573</v>
       </c>
       <c r="J3" s="1">
-        <v>29203.800061307847</v>
+        <v>525755.80204361677</v>
       </c>
       <c r="K3" s="1">
-        <v>283727.80040160567</v>
+        <v>29203.800039298832</v>
       </c>
       <c r="L3" s="1">
-        <v>285858.70012959838</v>
+        <v>283727.80025926977</v>
       </c>
       <c r="M3" s="1">
-        <v>200138.29981394112</v>
+        <v>285858.70011573285</v>
       </c>
       <c r="N3" s="1">
-        <v>34214.70003335923</v>
+        <v>200138.30009755492</v>
       </c>
       <c r="O3" s="1">
-        <v>279713.99981605262</v>
+        <v>34214.699999965727</v>
       </c>
       <c r="P3" s="1">
-        <v>273535.60060277581</v>
+        <v>279714.00009713322</v>
       </c>
       <c r="Q3" s="1">
-        <v>23499.100045084953</v>
+        <v>273535.6002253443</v>
       </c>
       <c r="R3" s="1">
-        <v>312931.60042268783</v>
+        <v>23499.100012376904</v>
       </c>
       <c r="S3" s="1">
-        <v>485996.99948277324</v>
+        <v>312931.60029856861</v>
       </c>
       <c r="T3" s="1">
-        <v>313928.69983317703</v>
+        <v>485997.00021328777</v>
       </c>
       <c r="U3" s="1">
-        <v>297034.70043640584</v>
+        <v>313928.70009709895</v>
+      </c>
+      <c r="V3" s="1">
+        <v>297034.7002377212</v>
       </c>
     </row>
     <row r="4">
@@ -324,64 +336,67 @@
         <v>1992</v>
       </c>
       <c r="B4" s="1">
-        <v>34028.89997445792</v>
+        <v>34028.899985261261</v>
       </c>
       <c r="C4" s="1">
-        <v>326180.80028748512</v>
+        <v>326180.80008783191</v>
       </c>
       <c r="D4" s="1">
-        <v>410724.00032814592</v>
+        <v>410724.00043000281</v>
       </c>
       <c r="E4" s="1">
-        <v>399704.90127181262</v>
+        <v>399704.90122456104</v>
       </c>
       <c r="F4" s="1">
-        <v>113724.40074580908</v>
+        <v>113724.400733307</v>
       </c>
       <c r="G4" s="1">
-        <v>179640.79995769262</v>
+        <v>179640.80003722757</v>
       </c>
       <c r="H4" s="1">
-        <v>408321.59979435056</v>
+        <v>408321.6000501439</v>
       </c>
       <c r="I4" s="1">
-        <v>63322.400301873684</v>
+        <v>63322.400341957808</v>
       </c>
       <c r="J4" s="1">
-        <v>28958.700062960386</v>
+        <v>534955.80212635547</v>
       </c>
       <c r="K4" s="1">
-        <v>281252.10037818551</v>
+        <v>28958.700038038194</v>
       </c>
       <c r="L4" s="1">
-        <v>283776.60011488944</v>
+        <v>281252.1002401337</v>
       </c>
       <c r="M4" s="1">
-        <v>198597.5997979939</v>
+        <v>283776.60009515285</v>
       </c>
       <c r="N4" s="1">
-        <v>33955.300028540194</v>
+        <v>198597.60008523613</v>
       </c>
       <c r="O4" s="1">
-        <v>278276.49980251491</v>
+        <v>33955.29999845475</v>
       </c>
       <c r="P4" s="1">
-        <v>272506.50057555735</v>
+        <v>278276.50008951873</v>
       </c>
       <c r="Q4" s="1">
-        <v>23368.700041651726</v>
+        <v>272506.50020512938</v>
       </c>
       <c r="R4" s="1">
-        <v>310210.80069301277</v>
+        <v>23368.700012274086</v>
       </c>
       <c r="S4" s="1">
-        <v>482374.19978109002</v>
+        <v>310210.8002781719</v>
       </c>
       <c r="T4" s="1">
-        <v>312231.80042778701</v>
+        <v>482374.20018038899</v>
       </c>
       <c r="U4" s="1">
-        <v>295875.20085892081</v>
+        <v>312231.80008797348</v>
+      </c>
+      <c r="V4" s="1">
+        <v>295875.20021740347</v>
       </c>
     </row>
     <row r="5">
@@ -389,64 +404,67 @@
         <v>1997</v>
       </c>
       <c r="B5" s="1">
-        <v>32694.799968130887</v>
+        <v>32694.799986936152</v>
       </c>
       <c r="C5" s="1">
-        <v>318596.90027798712</v>
+        <v>318596.90007647872</v>
       </c>
       <c r="D5" s="1">
-        <v>411963.70026227832</v>
+        <v>411963.70039319992</v>
       </c>
       <c r="E5" s="1">
-        <v>400059.90127716959</v>
+        <v>400059.90122722834</v>
       </c>
       <c r="F5" s="1">
-        <v>114703.30075372756</v>
+        <v>114703.30073112994</v>
       </c>
       <c r="G5" s="1">
-        <v>176979.79991899431</v>
+        <v>176979.79999534786</v>
       </c>
       <c r="H5" s="1">
-        <v>406921.39978945255</v>
+        <v>406921.40004363656</v>
       </c>
       <c r="I5" s="1">
-        <v>73728.000413887203</v>
+        <v>73728.000436335802</v>
       </c>
       <c r="J5" s="1">
-        <v>28614.100060492754</v>
+        <v>546260.80223190039</v>
       </c>
       <c r="K5" s="1">
-        <v>278231.90034101903</v>
+        <v>28614.100037030876</v>
       </c>
       <c r="L5" s="1">
-        <v>281246.70008831471</v>
+        <v>278231.90020880103</v>
       </c>
       <c r="M5" s="1">
-        <v>196635.19977666438</v>
+        <v>281246.70006889105</v>
       </c>
       <c r="N5" s="1">
-        <v>33697.600026026368</v>
+        <v>196635.20006649196</v>
       </c>
       <c r="O5" s="1">
-        <v>276691.09979146719</v>
+        <v>33697.599996343255</v>
       </c>
       <c r="P5" s="1">
-        <v>271132.90056282282</v>
+        <v>276691.10007810593</v>
       </c>
       <c r="Q5" s="1">
-        <v>23137.500039316714</v>
+        <v>271132.90019249916</v>
       </c>
       <c r="R5" s="1">
-        <v>306846.00032241642</v>
+        <v>23137.500010229647</v>
       </c>
       <c r="S5" s="1">
-        <v>477881.89992043376</v>
+        <v>306846.00024583191</v>
       </c>
       <c r="T5" s="1">
-        <v>310388.7001921609</v>
+        <v>477881.90013538301</v>
       </c>
       <c r="U5" s="1">
-        <v>294270.40080493689</v>
+        <v>310388.70007444918</v>
+      </c>
+      <c r="V5" s="1">
+        <v>294270.40020272881</v>
       </c>
     </row>
     <row r="6">
@@ -454,64 +472,67 @@
         <v>2002</v>
       </c>
       <c r="B6" s="1">
-        <v>31479.299961820245</v>
+        <v>31479.299977563322</v>
       </c>
       <c r="C6" s="1">
-        <v>303946.70026582479</v>
+        <v>303946.70005842298</v>
       </c>
       <c r="D6" s="1">
-        <v>412413.70020762086</v>
+        <v>412413.70034217089</v>
       </c>
       <c r="E6" s="1">
-        <v>401609.20130158961</v>
+        <v>401609.20124524087</v>
       </c>
       <c r="F6" s="1">
-        <v>115343.10075476021</v>
+        <v>115343.10073465854</v>
       </c>
       <c r="G6" s="1">
-        <v>182246.49990992248</v>
+        <v>182246.49998190254</v>
       </c>
       <c r="H6" s="1">
-        <v>406378.49974918365</v>
+        <v>406378.50002133101</v>
       </c>
       <c r="I6" s="1">
-        <v>82230.800510905683</v>
+        <v>82230.800529003143</v>
       </c>
       <c r="J6" s="1">
-        <v>28167.500054322183</v>
+        <v>557037.00235318393</v>
       </c>
       <c r="K6" s="1">
-        <v>275477.20031578839</v>
+        <v>28167.500035747886</v>
       </c>
       <c r="L6" s="1">
-        <v>278901.50006436557</v>
+        <v>275477.2001818344</v>
       </c>
       <c r="M6" s="1">
-        <v>195199.49975059181</v>
+        <v>278901.50004267693</v>
       </c>
       <c r="N6" s="1">
-        <v>33458.700022481382</v>
+        <v>195199.50004532933</v>
       </c>
       <c r="O6" s="1">
-        <v>275395.89978072792</v>
+        <v>33458.699993096292</v>
       </c>
       <c r="P6" s="1">
-        <v>268967.10051334649</v>
+        <v>275395.90006704628</v>
       </c>
       <c r="Q6" s="1">
-        <v>23043.400038696826</v>
+        <v>268967.10016188025</v>
       </c>
       <c r="R6" s="1">
-        <v>303644.70055441558</v>
+        <v>23043.400009498</v>
       </c>
       <c r="S6" s="1">
-        <v>474101.00040176511</v>
+        <v>303644.70021758229</v>
       </c>
       <c r="T6" s="1">
-        <v>308854.59972546995</v>
+        <v>474101.00008800626</v>
       </c>
       <c r="U6" s="1">
-        <v>292010.50020884722</v>
+        <v>308854.60006014258</v>
+      </c>
+      <c r="V6" s="1">
+        <v>292010.50017137825</v>
       </c>
     </row>
     <row r="7">
@@ -519,64 +540,67 @@
         <v>2007</v>
       </c>
       <c r="B7" s="1">
-        <v>32578.7999650985</v>
+        <v>32578.799973286688</v>
       </c>
       <c r="C7" s="1">
-        <v>298823.5002399534</v>
+        <v>298823.5000416711</v>
       </c>
       <c r="D7" s="1">
-        <v>412162.40016037226</v>
+        <v>412162.40030286461</v>
       </c>
       <c r="E7" s="1">
-        <v>402130.50130251795</v>
+        <v>402130.50124900788</v>
       </c>
       <c r="F7" s="1">
-        <v>117217.00075599551</v>
+        <v>117217.00073523819</v>
       </c>
       <c r="G7" s="1">
-        <v>179396.29990192503</v>
+        <v>179396.29996844381</v>
       </c>
       <c r="H7" s="1">
-        <v>405568.39974284917</v>
+        <v>405568.40001321584</v>
       </c>
       <c r="I7" s="1">
-        <v>87770.900592915714</v>
+        <v>87770.900606565177</v>
       </c>
       <c r="J7" s="1">
-        <v>27857.100053675473</v>
+        <v>563588.90244240314</v>
       </c>
       <c r="K7" s="1">
-        <v>273569.40028021485</v>
+        <v>27857.100032843649</v>
       </c>
       <c r="L7" s="1">
-        <v>277538.100043796</v>
+        <v>273569.40015505999</v>
       </c>
       <c r="M7" s="1">
-        <v>194130.29973341525</v>
+        <v>277538.1000245139</v>
       </c>
       <c r="N7" s="1">
-        <v>33300.300020866096</v>
+        <v>194130.30003011227</v>
       </c>
       <c r="O7" s="1">
-        <v>274717.89976213127</v>
+        <v>33300.2999914065</v>
       </c>
       <c r="P7" s="1">
-        <v>267977.70051269233</v>
+        <v>274717.9000524655</v>
       </c>
       <c r="Q7" s="1">
-        <v>22968.100036777556</v>
+        <v>267977.7001529038</v>
       </c>
       <c r="R7" s="1">
-        <v>301426.50051239133</v>
+        <v>22968.100008584559</v>
       </c>
       <c r="S7" s="1">
-        <v>471668.39942433685</v>
+        <v>301426.50018790364</v>
       </c>
       <c r="T7" s="1">
-        <v>308018.19972027093</v>
+        <v>471668.40005462617</v>
       </c>
       <c r="U7" s="1">
-        <v>290945.80068060756</v>
+        <v>308018.200043872</v>
+      </c>
+      <c r="V7" s="1">
+        <v>290945.80016148835</v>
       </c>
     </row>
     <row r="8">
@@ -584,64 +608,67 @@
         <v>2012</v>
       </c>
       <c r="B8" s="1">
-        <v>23949.599969789386</v>
+        <v>23949.599979385734</v>
       </c>
       <c r="C8" s="1">
-        <v>307765.8002416268</v>
+        <v>307765.80003920197</v>
       </c>
       <c r="D8" s="1">
-        <v>412705.60012216866</v>
+        <v>412705.6002696529</v>
       </c>
       <c r="E8" s="1">
-        <v>402616.90131063014</v>
+        <v>402616.90125477314</v>
       </c>
       <c r="F8" s="1">
-        <v>118212.60076145828</v>
+        <v>118212.60073700547</v>
       </c>
       <c r="G8" s="1">
-        <v>175692.29988637567</v>
+        <v>175692.29995437711</v>
       </c>
       <c r="H8" s="1">
-        <v>404044.5997281298</v>
+        <v>404044.60000356287</v>
       </c>
       <c r="I8" s="1">
-        <v>90660.400641448796</v>
+        <v>90660.400652334094</v>
       </c>
       <c r="J8" s="1">
-        <v>27692.400049224496</v>
+        <v>567276.10249810666</v>
       </c>
       <c r="K8" s="1">
-        <v>272671.80026450753</v>
+        <v>27692.400029584765</v>
       </c>
       <c r="L8" s="1">
-        <v>276709.90002723038</v>
+        <v>272671.80014347285</v>
       </c>
       <c r="M8" s="1">
-        <v>193570.89972167462</v>
+        <v>276709.90000744909</v>
       </c>
       <c r="N8" s="1">
-        <v>33232.800019867718</v>
+        <v>193570.90002006292</v>
       </c>
       <c r="O8" s="1">
-        <v>274218.79975289851</v>
+        <v>33232.799990147352</v>
       </c>
       <c r="P8" s="1">
-        <v>267305.10050263256</v>
+        <v>274218.80004697293</v>
       </c>
       <c r="Q8" s="1">
-        <v>22970.000036463141</v>
+        <v>267305.10014606267</v>
       </c>
       <c r="R8" s="1">
-        <v>300364.2005763948</v>
+        <v>22970.000008434057</v>
       </c>
       <c r="S8" s="1">
-        <v>470280.80000023544</v>
+        <v>300364.20017305762</v>
       </c>
       <c r="T8" s="1">
-        <v>307451.59990778565</v>
+        <v>470280.80002751201</v>
       </c>
       <c r="U8" s="1">
-        <v>290275.10016013682</v>
+        <v>307451.60003712028</v>
+      </c>
+      <c r="V8" s="1">
+        <v>290275.10015449673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AT: revise land use class data source to "broad" variable
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/combined/landu_lcc_totalarea.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>year</t>
   </si>
@@ -24,22 +24,25 @@
     <t>Cropland_acresk</t>
   </si>
   <si>
+    <t>Federalland_acresk</t>
+  </si>
+  <si>
     <t>Forestland_acresk</t>
   </si>
   <si>
-    <t>NAland_acresk</t>
-  </si>
-  <si>
-    <t>Otherland_acresk</t>
-  </si>
-  <si>
     <t>Pastureland_acresk</t>
   </si>
   <si>
     <t>Rangeland_acresk</t>
   </si>
   <si>
+    <t>Ruralland_acresk</t>
+  </si>
+  <si>
     <t>Urbanland_acresk</t>
+  </si>
+  <si>
+    <t>Waterland_acresk</t>
   </si>
   <si>
     <t>lccNA_acresk</t>
@@ -124,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:W8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -194,6 +197,9 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -203,63 +209,66 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>366293.8001255244</v>
+        <v>419711.70014646649</v>
       </c>
       <c r="D2" s="1">
+        <v>397162.801202178</v>
+      </c>
+      <c r="E2" s="1">
         <v>408769.80048586428</v>
       </c>
-      <c r="E2" s="1">
-        <v>397162.801202178</v>
-      </c>
       <c r="F2" s="1">
-        <v>112054.60071638972</v>
+        <v>130264.90003698319</v>
       </c>
       <c r="G2" s="1">
-        <v>183682.80005792528</v>
+        <v>417288.50006688386</v>
       </c>
       <c r="H2" s="1">
-        <v>417288.50006688386</v>
+        <v>62501.500497281551</v>
       </c>
       <c r="I2" s="1">
         <v>50395.500235527754</v>
       </c>
       <c r="J2" s="1">
+        <v>49553.100219108164</v>
+      </c>
+      <c r="K2" s="1">
         <v>518365.7019867152</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>29415.90003991127</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>285804.70027589798</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>287258.20012904704</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>201368.20010298491</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>34436.700000435114</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>280848.30010822415</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>274476.90023375303</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>23673.200013324618</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>315220.60031580925</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>488626.40023203194</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>315285.00010865927</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>298150.10024707764</v>
       </c>
     </row>
@@ -271,63 +280,66 @@
         <v>13776.79998434335</v>
       </c>
       <c r="C3" s="1">
-        <v>347130.90011132509</v>
+        <v>405583.60013335943</v>
       </c>
       <c r="D3" s="1">
+        <v>397583.60121012479</v>
+      </c>
+      <c r="E3" s="1">
         <v>410698.3004591614</v>
       </c>
-      <c r="E3" s="1">
-        <v>397583.60121012479</v>
-      </c>
       <c r="F3" s="1">
-        <v>113429.90072029084</v>
+        <v>126303.40002986044</v>
       </c>
       <c r="G3" s="1">
-        <v>184756.10005189478</v>
+        <v>411972.80007003248</v>
       </c>
       <c r="H3" s="1">
-        <v>411972.80007003248</v>
+        <v>62871.700501479208</v>
       </c>
       <c r="I3" s="1">
         <v>56299.400283120573</v>
       </c>
       <c r="J3" s="1">
+        <v>50558.200218811631</v>
+      </c>
+      <c r="K3" s="1">
         <v>525755.80204361677</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>29203.800039298832</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>283727.80025926977</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>285858.70011573285</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>200138.30009755492</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>34214.699999965727</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>279714.00009713322</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>273535.6002253443</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>23499.100012376904</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>312931.60029856861</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>485997.00021328777</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>313928.70009709895</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>297034.7002377212</v>
       </c>
     </row>
@@ -339,63 +351,66 @@
         <v>34028.899985261261</v>
       </c>
       <c r="C4" s="1">
-        <v>326180.80008783191</v>
+        <v>381450.30009821802</v>
       </c>
       <c r="D4" s="1">
+        <v>399704.90122456104</v>
+      </c>
+      <c r="E4" s="1">
         <v>410724.00043000281</v>
       </c>
-      <c r="E4" s="1">
-        <v>399704.90122456104</v>
-      </c>
       <c r="F4" s="1">
-        <v>113724.400733307</v>
+        <v>124371.30002684146</v>
       </c>
       <c r="G4" s="1">
-        <v>179640.80003722757</v>
+        <v>408321.6000501439</v>
       </c>
       <c r="H4" s="1">
-        <v>408321.6000501439</v>
+        <v>63256.500508159399</v>
       </c>
       <c r="I4" s="1">
         <v>63322.400341957808</v>
       </c>
       <c r="J4" s="1">
+        <v>50467.900225147605</v>
+      </c>
+      <c r="K4" s="1">
         <v>534955.80212635547</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>28958.700038038194</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>281252.1002401337</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>283776.60009515285</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>198597.60008523613</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>33955.29999845475</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>278276.50008951873</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>272506.50020512938</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>23368.700012274086</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>310210.8002781719</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>482374.20018038899</v>
       </c>
-      <c r="U4" s="1">
+      <c r="V4" s="1">
         <v>312231.80008797348</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>295875.20021740347</v>
       </c>
     </row>
@@ -407,63 +422,66 @@
         <v>32694.799986936152</v>
       </c>
       <c r="C5" s="1">
-        <v>318596.90007647872</v>
+        <v>375864.00007351488</v>
       </c>
       <c r="D5" s="1">
+        <v>400059.90122722834</v>
+      </c>
+      <c r="E5" s="1">
         <v>411963.70039319992</v>
       </c>
-      <c r="E5" s="1">
-        <v>400059.90122722834</v>
-      </c>
       <c r="F5" s="1">
-        <v>114703.30073112994</v>
+        <v>119712.6999983117</v>
       </c>
       <c r="G5" s="1">
-        <v>176979.79999534786</v>
+        <v>406921.40004363656</v>
       </c>
       <c r="H5" s="1">
-        <v>406921.40004363656</v>
+        <v>63888.200500778854</v>
       </c>
       <c r="I5" s="1">
         <v>73728.000436335802</v>
       </c>
       <c r="J5" s="1">
+        <v>50815.10023035109</v>
+      </c>
+      <c r="K5" s="1">
         <v>546260.80223190039</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>28614.100037030876</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>278231.90020880103</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>281246.70006889105</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>196635.20006649196</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>33697.599996343255</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>276691.10007810593</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>271132.90019249916</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>23137.500010229647</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>306846.00024583191</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>477881.90013538301</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V5" s="1">
         <v>310388.70007444918</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W5" s="1">
         <v>294270.40020272881</v>
       </c>
     </row>
@@ -475,63 +493,66 @@
         <v>31479.299977563322</v>
       </c>
       <c r="C6" s="1">
-        <v>303946.70005842298</v>
+        <v>367470.50004819036</v>
       </c>
       <c r="D6" s="1">
+        <v>401609.20124524087</v>
+      </c>
+      <c r="E6" s="1">
         <v>412413.70034217089</v>
       </c>
-      <c r="E6" s="1">
-        <v>401609.20124524087</v>
-      </c>
       <c r="F6" s="1">
-        <v>115343.10073465854</v>
+        <v>118722.69999213517</v>
       </c>
       <c r="G6" s="1">
-        <v>182246.49998190254</v>
+        <v>406378.50002133101</v>
       </c>
       <c r="H6" s="1">
-        <v>406378.50002133101</v>
+        <v>64069.800497464836</v>
       </c>
       <c r="I6" s="1">
         <v>82230.800529003143</v>
       </c>
       <c r="J6" s="1">
+        <v>51273.300237193704</v>
+      </c>
+      <c r="K6" s="1">
         <v>557037.00235318393</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>28167.500035747886</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>275477.2001818344</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>278901.50004267693</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>195199.50004532933</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>33458.699993096292</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>275395.90006704628</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <v>268967.10016188025</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>23043.400009498</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>303644.70021758229</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>474101.00008800626</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <v>308854.60006014258</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W6" s="1">
         <v>292010.50017137825</v>
       </c>
     </row>
@@ -543,63 +564,66 @@
         <v>32578.799973286688</v>
       </c>
       <c r="C7" s="1">
-        <v>298823.5000416711</v>
+        <v>358786.00003223866</v>
       </c>
       <c r="D7" s="1">
+        <v>402130.50124900788</v>
+      </c>
+      <c r="E7" s="1">
         <v>412162.40030286461</v>
       </c>
-      <c r="E7" s="1">
-        <v>402130.50124900788</v>
-      </c>
       <c r="F7" s="1">
-        <v>117217.00073523819</v>
+        <v>119433.79997787625</v>
       </c>
       <c r="G7" s="1">
-        <v>179396.29996844381</v>
+        <v>405568.40001321584</v>
       </c>
       <c r="H7" s="1">
-        <v>405568.40001321584</v>
+        <v>65602.700492627919</v>
       </c>
       <c r="I7" s="1">
         <v>87770.900606565177</v>
       </c>
       <c r="J7" s="1">
+        <v>51614.300242610276</v>
+      </c>
+      <c r="K7" s="1">
         <v>563588.90244240314</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>27857.100032843649</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>273569.40015505999</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>277538.1000245139</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>194130.30003011227</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>33300.2999914065</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>274717.9000524655</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>267977.7001529038</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>22968.100008584559</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>301426.50018790364</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>471668.40005462617</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>308018.200043872</v>
       </c>
-      <c r="V7" s="1">
+      <c r="W7" s="1">
         <v>290945.80016148835</v>
       </c>
     </row>
@@ -611,63 +635,66 @@
         <v>23949.599979385734</v>
       </c>
       <c r="C8" s="1">
-        <v>307765.80003920197</v>
+        <v>361765.00001784414</v>
       </c>
       <c r="D8" s="1">
+        <v>402616.90125477314</v>
+      </c>
+      <c r="E8" s="1">
         <v>412705.6002696529</v>
       </c>
-      <c r="E8" s="1">
-        <v>402616.90125477314</v>
-      </c>
       <c r="F8" s="1">
-        <v>118212.60073700547</v>
+        <v>121693.09997573495</v>
       </c>
       <c r="G8" s="1">
-        <v>175692.29995437711</v>
+        <v>404044.60000356287</v>
       </c>
       <c r="H8" s="1">
-        <v>404044.60000356287</v>
+        <v>66392.200491629541</v>
       </c>
       <c r="I8" s="1">
         <v>90660.400652334094</v>
       </c>
       <c r="J8" s="1">
+        <v>51820.400245375931</v>
+      </c>
+      <c r="K8" s="1">
         <v>567276.10249810666</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>27692.400029584765</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>272671.80014347285</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>276709.90000744909</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>193570.90002006292</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>33232.799990147352</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q8" s="1">
         <v>274218.80004697293</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>267305.10014606267</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>22970.000008434057</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>300364.20017305762</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>470280.80002751201</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <v>307451.60003712028</v>
       </c>
-      <c r="V8" s="1">
+      <c r="W8" s="1">
         <v>290275.10015449673</v>
       </c>
     </row>

</xml_diff>